<commit_message>
Adding to the impact information profiles & finalising the GCDB_table object
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -20,51 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="140">
   <si>
     <t xml:space="preserve">imp_src_orgtype</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">imp_</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">src_org</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">imp_</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">src_db</t>
-    </r>
+    <t xml:space="preserve">imp_src_org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imp_src_db</t>
   </si>
   <si>
     <t xml:space="preserve">VarName</t>
@@ -73,66 +37,10 @@
     <t xml:space="preserve">imp_cats</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">imp</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">subcats</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">imp</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">det</t>
-    </r>
+    <t xml:space="preserve">imp_subcats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imp_det</t>
   </si>
   <si>
     <t xml:space="preserve">imp_units</t>
@@ -171,7 +79,7 @@
     <t xml:space="preserve">imptypdeat</t>
   </si>
   <si>
-    <t xml:space="preserve">impobsest</t>
+    <t xml:space="preserve">esttype_prim</t>
   </si>
   <si>
     <t xml:space="preserve">injured</t>
@@ -514,6 +422,24 @@
   </si>
   <si>
     <t xml:space="preserve">gdacs_alertscore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imptyperisk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impdetalert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitsgdacsalert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imptypalert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esttype_model</t>
   </si>
 </sst>
 </file>
@@ -553,12 +479,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -575,6 +495,13 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Calibri&quot;"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -646,11 +573,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -658,7 +581,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -666,20 +589,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -761,8 +688,8 @@
   </sheetPr>
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G61" activeCellId="0" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -770,9 +697,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.16"/>
@@ -784,10 +711,10 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -813,7 +740,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -825,19 +752,19 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -845,31 +772,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -877,31 +804,31 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -909,31 +836,31 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -941,31 +868,31 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -973,7 +900,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -985,19 +912,19 @@
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -1005,31 +932,31 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1037,31 +964,31 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="4" t="s">
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -1069,31 +996,31 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -1101,31 +1028,31 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1133,7 +1060,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1145,17 +1072,17 @@
       <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="4" t="s">
+      <c r="H12" s="6"/>
+      <c r="I12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1163,31 +1090,31 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="H13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>50</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -1195,31 +1122,31 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="4" t="s">
+      <c r="H14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>50</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -1227,31 +1154,31 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -1259,31 +1186,31 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="4" t="s">
+      <c r="H16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -1291,31 +1218,31 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
@@ -1323,31 +1250,31 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1355,7 +1282,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1367,19 +1294,19 @@
       <c r="D19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="4" t="s">
+      <c r="E19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="1" t="s">
@@ -1387,31 +1314,31 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="E20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="J20" s="1" t="s">
@@ -1419,31 +1346,31 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="4" t="s">
+      <c r="E21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>75</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1451,31 +1378,31 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="4" t="s">
+      <c r="E22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>77</v>
       </c>
       <c r="J22" s="1" t="s">
@@ -1483,7 +1410,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1495,19 +1422,19 @@
       <c r="D23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="4" t="s">
+      <c r="E23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>79</v>
       </c>
       <c r="J23" s="1" t="s">
@@ -1515,31 +1442,31 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J24" s="1" t="s">
@@ -1547,31 +1474,31 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J25" s="1" t="s">
@@ -1579,31 +1506,31 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J26" s="1" t="s">
@@ -1611,7 +1538,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1623,19 +1550,19 @@
       <c r="D27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J27" s="1" t="s">
@@ -1643,31 +1570,31 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J28" s="1" t="s">
@@ -1675,31 +1602,31 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J29" s="1" t="s">
@@ -1707,31 +1634,31 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="4" t="s">
+      <c r="E30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>95</v>
       </c>
       <c r="J30" s="1" t="s">
@@ -1739,7 +1666,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1751,19 +1678,19 @@
       <c r="D31" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="9" t="s">
+      <c r="E31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="8" t="s">
         <v>99</v>
       </c>
       <c r="J31" s="1" t="s">
@@ -1771,7 +1698,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1783,19 +1710,19 @@
       <c r="D32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="8" t="s">
         <v>102</v>
       </c>
       <c r="J32" s="1" t="s">
@@ -1803,7 +1730,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1815,19 +1742,19 @@
       <c r="D33" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="8" t="s">
         <v>104</v>
       </c>
       <c r="J33" s="1" t="s">
@@ -1835,7 +1762,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1847,19 +1774,19 @@
       <c r="D34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="4" t="s">
+      <c r="E34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>21</v>
       </c>
       <c r="J34" s="1" t="s">
@@ -1867,7 +1794,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1879,19 +1806,19 @@
       <c r="D35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="4" t="s">
+      <c r="E35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J35" s="1" t="s">
@@ -1899,7 +1826,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1911,19 +1838,19 @@
       <c r="D36" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="4" t="s">
+      <c r="E36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J36" s="1" t="s">
@@ -1931,7 +1858,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1943,19 +1870,19 @@
       <c r="D37" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="4" t="s">
+      <c r="E37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>79</v>
       </c>
       <c r="J37" s="1" t="s">
@@ -1963,7 +1890,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1975,19 +1902,19 @@
       <c r="D38" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="11" t="s">
+      <c r="E38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" s="10" t="s">
         <v>111</v>
       </c>
       <c r="J38" s="1" t="s">
@@ -1995,7 +1922,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2007,19 +1934,19 @@
       <c r="D39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="11" t="s">
+      <c r="E39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="10" t="s">
         <v>113</v>
       </c>
       <c r="J39" s="1" t="s">
@@ -2027,7 +1954,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2039,19 +1966,19 @@
       <c r="D40" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" s="4" t="s">
+      <c r="E40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>21</v>
       </c>
       <c r="J40" s="1" t="s">
@@ -2059,7 +1986,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2071,19 +1998,19 @@
       <c r="D41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="4" t="s">
+      <c r="E41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J41" s="1" t="s">
@@ -2091,7 +2018,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2103,19 +2030,19 @@
       <c r="D42" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I42" s="4" t="s">
+      <c r="E42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J42" s="1" t="s">
@@ -2123,7 +2050,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2135,19 +2062,19 @@
       <c r="D43" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" s="4" t="s">
+      <c r="E43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>79</v>
       </c>
       <c r="J43" s="1" t="s">
@@ -2155,7 +2082,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2167,19 +2094,19 @@
       <c r="D44" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" s="11" t="s">
+      <c r="E44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="10" t="s">
         <v>111</v>
       </c>
       <c r="J44" s="1" t="s">
@@ -2187,7 +2114,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2199,19 +2126,19 @@
       <c r="D45" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I45" s="11" t="s">
+      <c r="E45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="10" t="s">
         <v>113</v>
       </c>
       <c r="J45" s="1" t="s">
@@ -2219,7 +2146,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2231,19 +2158,19 @@
       <c r="D46" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I46" s="4" t="s">
+      <c r="E46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="3" t="s">
         <v>21</v>
       </c>
       <c r="J46" s="1" t="s">
@@ -2251,7 +2178,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2263,19 +2190,19 @@
       <c r="D47" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="4" t="s">
+      <c r="E47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J47" s="1" t="s">
@@ -2283,7 +2210,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2295,19 +2222,19 @@
       <c r="D48" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I48" s="4" t="s">
+      <c r="E48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J48" s="1" t="s">
@@ -2315,7 +2242,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2327,19 +2254,19 @@
       <c r="D49" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I49" s="4" t="s">
+      <c r="E49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" s="3" t="s">
         <v>79</v>
       </c>
       <c r="J49" s="1" t="s">
@@ -2347,7 +2274,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2359,19 +2286,19 @@
       <c r="D50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I50" s="11" t="s">
+      <c r="E50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="10" t="s">
         <v>111</v>
       </c>
       <c r="J50" s="1" t="s">
@@ -2379,7 +2306,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2391,19 +2318,19 @@
       <c r="D51" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I51" s="11" t="s">
+      <c r="E51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" s="10" t="s">
         <v>113</v>
       </c>
       <c r="J51" s="1" t="s">
@@ -2411,7 +2338,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2423,7 +2350,7 @@
       <c r="D52" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H52" s="10" t="s">
+      <c r="H52" s="9" t="s">
         <v>101</v>
       </c>
       <c r="J52" s="1" t="s">
@@ -2431,7 +2358,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2443,7 +2370,7 @@
       <c r="D53" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H53" s="10" t="s">
+      <c r="H53" s="9" t="s">
         <v>101</v>
       </c>
       <c r="J53" s="1" t="s">
@@ -2451,7 +2378,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2463,7 +2390,7 @@
       <c r="D54" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H54" s="9" t="s">
         <v>101</v>
       </c>
       <c r="J54" s="1" t="s">
@@ -2471,7 +2398,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2483,7 +2410,7 @@
       <c r="D55" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H55" s="10" t="s">
+      <c r="H55" s="9" t="s">
         <v>101</v>
       </c>
       <c r="J55" s="1" t="s">
@@ -2491,7 +2418,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="8" t="s">
         <v>130</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2502,6 +2429,24 @@
       </c>
       <c r="D56" s="1" t="s">
         <v>133</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Next stage of the database re-write. Potential issues to be faced due to refactorisation of many of the database features. Some files were not repaired, such as all those in the Analysis folder.
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -34,10 +34,10 @@
     <t xml:space="preserve">VarName</t>
   </si>
   <si>
-    <t xml:space="preserve">imp_cats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imp_subcats</t>
+    <t xml:space="preserve">imp_cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imp_subcat</t>
   </si>
   <si>
     <t xml:space="preserve">imp_det</t>
@@ -688,8 +688,8 @@
   </sheetPr>
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G61" activeCellId="0" sqref="G61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updating the JSON schema, again ...sigh...
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="140">
   <si>
     <t xml:space="preserve">imp_src_orgtype</t>
   </si>
@@ -34,13 +34,13 @@
     <t xml:space="preserve">VarName</t>
   </si>
   <si>
-    <t xml:space="preserve">imp_cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imp_subcat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imp_det</t>
+    <t xml:space="preserve">exp_cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp_subcat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp_spec</t>
   </si>
   <si>
     <t xml:space="preserve">imp_units</t>
@@ -64,13 +64,13 @@
     <t xml:space="preserve">deaths</t>
   </si>
   <si>
-    <t xml:space="preserve">impcatpop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imptypepopcnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetallpeop</t>
+    <t xml:space="preserve">expcat_pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expsubcat_popcnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_allpeop</t>
   </si>
   <si>
     <t xml:space="preserve">unitscountnum</t>
@@ -97,13 +97,13 @@
     <t xml:space="preserve">houses_destroyed</t>
   </si>
   <si>
-    <t xml:space="preserve">impcatphyinf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impinftot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetbuild</t>
+    <t xml:space="preserve">expcat_phyinf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expsubcat_inftot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_build</t>
   </si>
   <si>
     <t xml:space="preserve">imptypdest</t>
@@ -142,13 +142,13 @@
     <t xml:space="preserve">losses_in_dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">impcatfineco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impecotot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetusdunsure</t>
+    <t xml:space="preserve">expcat_fineco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expsubcat_ecotot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_usdunsure</t>
   </si>
   <si>
     <t xml:space="preserve">unitISO4217C-USD</t>
@@ -160,16 +160,16 @@
     <t xml:space="preserve">losses_local_currency</t>
   </si>
   <si>
-    <t xml:space="preserve">impdetloccur</t>
+    <t xml:space="preserve">expspec_loccur</t>
   </si>
   <si>
     <t xml:space="preserve">education_centers</t>
   </si>
   <si>
-    <t xml:space="preserve">impphyedu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdeteduc</t>
+    <t xml:space="preserve">expsubcat_phyedu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_educ</t>
   </si>
   <si>
     <t xml:space="preserve">imptypunspec</t>
@@ -178,22 +178,22 @@
     <t xml:space="preserve">hospitals</t>
   </si>
   <si>
-    <t xml:space="preserve">impphyhealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdethosp</t>
+    <t xml:space="preserve">expsubcat_phyhealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_hosp</t>
   </si>
   <si>
     <t xml:space="preserve">damages_in_crops_ha</t>
   </si>
   <si>
-    <t xml:space="preserve">impcatenv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impinfarabl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetcrop</t>
+    <t xml:space="preserve">expcat_env</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expsubcat_infarabl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_crop</t>
   </si>
   <si>
     <t xml:space="preserve">unitshectare</t>
@@ -202,19 +202,19 @@
     <t xml:space="preserve">lost_cattle</t>
   </si>
   <si>
-    <t xml:space="preserve">impenvliv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetcattle</t>
+    <t xml:space="preserve">expsubcat_envliv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_cattle</t>
   </si>
   <si>
     <t xml:space="preserve">damages_in_roads_mts</t>
   </si>
   <si>
-    <t xml:space="preserve">impinfrds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetroad</t>
+    <t xml:space="preserve">expsubcat_infrds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_road</t>
   </si>
   <si>
     <t xml:space="preserve">unitsm</t>
@@ -232,10 +232,10 @@
     <t xml:space="preserve">AID.Contribution</t>
   </si>
   <si>
-    <t xml:space="preserve">impecoaid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetaidgen</t>
+    <t xml:space="preserve">expsubcat_ecoaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_aidgen</t>
   </si>
   <si>
     <t xml:space="preserve">Total.Deaths</t>
@@ -265,22 +265,22 @@
     <t xml:space="preserve">Reconstruction.Costs</t>
   </si>
   <si>
-    <t xml:space="preserve">impdetreccost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetinfloccur</t>
+    <t xml:space="preserve">expsubcat_detreccost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_infloccur</t>
   </si>
   <si>
     <t xml:space="preserve">Reconstruction.Costs.Adjusted</t>
   </si>
   <si>
-    <t xml:space="preserve">impdetinfglobdate</t>
+    <t xml:space="preserve">expspec_infglobdate</t>
   </si>
   <si>
     <t xml:space="preserve">Insured.Damages</t>
   </si>
   <si>
-    <t xml:space="preserve">impecoins</t>
+    <t xml:space="preserve">expsubcat_ecoins</t>
   </si>
   <si>
     <t xml:space="preserve">Insured.Damages.Adjusted</t>
@@ -289,7 +289,7 @@
     <t xml:space="preserve">Total.Damages</t>
   </si>
   <si>
-    <t xml:space="preserve">impecodirtot</t>
+    <t xml:space="preserve">expsubcat_ecodirtot</t>
   </si>
   <si>
     <t xml:space="preserve">Total.Damages.Adjusted</t>
@@ -424,13 +424,13 @@
     <t xml:space="preserve">gdacs_alertscore</t>
   </si>
   <si>
-    <t xml:space="preserve">impother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imptyperisk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impdetalert</t>
+    <t xml:space="preserve">expcat_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expsubcat_risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expspec_alert</t>
   </si>
   <si>
     <t xml:space="preserve">unitsgdacsalert</t>
@@ -689,7 +689,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -698,9 +698,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.28"/>
@@ -2350,6 +2350,15 @@
       <c r="D52" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="E52" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="H52" s="9" t="s">
         <v>101</v>
       </c>
@@ -2370,6 +2379,15 @@
       <c r="D53" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="E53" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="H53" s="9" t="s">
         <v>101</v>
       </c>
@@ -2390,6 +2408,15 @@
       <c r="D54" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="E54" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="H54" s="9" t="s">
         <v>101</v>
       </c>
@@ -2409,6 +2436,15 @@
       </c>
       <c r="D55" s="1" t="s">
         <v>129</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Many modifications to allow for the conversion between Monty JSON object into a tabular geospatial object format.
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -325,16 +325,16 @@
     <t xml:space="preserve">amount_requested</t>
   </si>
   <si>
+    <t xml:space="preserve">expspec_ecoifrcreq</t>
+  </si>
+  <si>
     <t xml:space="preserve">unitISO4217C-CHF</t>
   </si>
   <si>
-    <t xml:space="preserve">imptypaidreqifrc</t>
-  </si>
-  <si>
     <t xml:space="preserve">amount_funded</t>
   </si>
   <si>
-    <t xml:space="preserve">imptypaidallifrc</t>
+    <t xml:space="preserve">expspec_ecoifrcall</t>
   </si>
   <si>
     <t xml:space="preserve">GO-FR</t>
@@ -449,7 +449,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -489,6 +489,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -560,7 +567,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -598,6 +605,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -605,7 +616,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -689,7 +700,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1716,14 +1727,14 @@
       <c r="F32" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H32" s="9" t="s">
+      <c r="G32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="H32" s="10" t="s">
         <v>102</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>19</v>
@@ -1748,14 +1759,14 @@
       <c r="F33" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I33" s="8" t="s">
+      <c r="G33" s="9" t="s">
         <v>104</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>19</v>
@@ -1914,7 +1925,7 @@
       <c r="H38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="11" t="s">
         <v>111</v>
       </c>
       <c r="J38" s="1" t="s">
@@ -1946,7 +1957,7 @@
       <c r="H39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I39" s="10" t="s">
+      <c r="I39" s="11" t="s">
         <v>113</v>
       </c>
       <c r="J39" s="1" t="s">
@@ -2106,7 +2117,7 @@
       <c r="H44" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="10" t="s">
+      <c r="I44" s="11" t="s">
         <v>111</v>
       </c>
       <c r="J44" s="1" t="s">
@@ -2138,7 +2149,7 @@
       <c r="H45" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I45" s="10" t="s">
+      <c r="I45" s="11" t="s">
         <v>113</v>
       </c>
       <c r="J45" s="1" t="s">
@@ -2298,7 +2309,7 @@
       <c r="H50" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I50" s="10" t="s">
+      <c r="I50" s="11" t="s">
         <v>111</v>
       </c>
       <c r="J50" s="1" t="s">
@@ -2330,7 +2341,7 @@
       <c r="H51" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I51" s="10" t="s">
+      <c r="I51" s="11" t="s">
         <v>113</v>
       </c>
       <c r="J51" s="1" t="s">
@@ -2359,8 +2370,8 @@
       <c r="G52" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H52" s="9" t="s">
-        <v>101</v>
+      <c r="H52" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>19</v>
@@ -2388,8 +2399,8 @@
       <c r="G53" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H53" s="9" t="s">
-        <v>101</v>
+      <c r="H53" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>19</v>
@@ -2417,8 +2428,8 @@
       <c r="G54" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H54" s="9" t="s">
-        <v>101</v>
+      <c r="H54" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>19</v>
@@ -2446,8 +2457,8 @@
       <c r="G55" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H55" s="9" t="s">
-        <v>101</v>
+      <c r="H55" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>19</v>
@@ -2469,7 +2480,7 @@
       <c r="E56" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F56" s="11" t="s">
+      <c r="F56" s="12" t="s">
         <v>135</v>
       </c>
       <c r="G56" s="7" t="s">

</xml_diff>

<commit_message>
Adding GIDD and IDU databases to Monty, in the correct format/structure
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="149">
   <si>
     <t xml:space="preserve">imp_src_orgtype</t>
   </si>
@@ -154,6 +154,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">expspec_ecotot</t>
     </r>
@@ -339,6 +340,18 @@
     <t xml:space="preserve">imptypidp</t>
   </si>
   <si>
+    <t xml:space="preserve">new_displacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_displacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figure</t>
+  </si>
+  <si>
     <t xml:space="preserve">IFRC</t>
   </si>
   <si>
@@ -481,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -522,12 +535,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -599,7 +606,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,7 +635,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -640,15 +647,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -656,7 +659,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -737,10 +740,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C18:C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1513,7 +1516,7 @@
       <c r="F24" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="6" t="s">
         <v>82</v>
       </c>
       <c r="H24" s="3" t="s">
@@ -1545,7 +1548,7 @@
       <c r="F25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="6" t="s">
         <v>84</v>
       </c>
       <c r="H25" s="3" t="s">
@@ -1722,29 +1725,29 @@
       <c r="A31" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="E31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="11" t="s">
-        <v>103</v>
+      <c r="I31" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>19</v>
@@ -1754,29 +1757,29 @@
       <c r="A32" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>106</v>
+        <v>14</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>19</v>
@@ -1786,29 +1789,29 @@
       <c r="A33" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>101</v>
+      <c r="B33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>106</v>
+        <v>14</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>19</v>
@@ -1819,13 +1822,13 @@
         <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>14</v>
@@ -1833,14 +1836,14 @@
       <c r="F34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>21</v>
+      <c r="I34" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>19</v>
@@ -1851,28 +1854,28 @@
         <v>95</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>17</v>
+      <c r="H35" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>19</v>
@@ -1883,28 +1886,28 @@
         <v>95</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>17</v>
+      <c r="H36" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>19</v>
@@ -1915,13 +1918,13 @@
         <v>95</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>14</v>
@@ -1936,7 +1939,7 @@
         <v>17</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>19</v>
@@ -1947,13 +1950,13 @@
         <v>95</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>14</v>
@@ -1967,22 +1970,22 @@
       <c r="H38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I38" s="13" t="s">
-        <v>115</v>
+      <c r="I38" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>116</v>
@@ -1993,14 +1996,14 @@
       <c r="F39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I39" s="13" t="s">
-        <v>117</v>
+      <c r="I39" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>19</v>
@@ -2011,13 +2014,13 @@
         <v>95</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>14</v>
@@ -2032,7 +2035,7 @@
         <v>17</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>19</v>
@@ -2043,42 +2046,42 @@
         <v>95</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="J41" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>120</v>
@@ -2089,14 +2092,14 @@
       <c r="F42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I42" s="3" t="s">
-        <v>23</v>
+      <c r="I42" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>19</v>
@@ -2107,13 +2110,13 @@
         <v>95</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>14</v>
@@ -2128,7 +2131,7 @@
         <v>17</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>19</v>
@@ -2139,13 +2142,13 @@
         <v>95</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>14</v>
@@ -2159,25 +2162,25 @@
       <c r="H44" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="13" t="s">
-        <v>115</v>
+      <c r="I44" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>14</v>
@@ -2185,14 +2188,14 @@
       <c r="F45" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I45" s="13" t="s">
-        <v>117</v>
+      <c r="I45" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>19</v>
@@ -2203,13 +2206,13 @@
         <v>95</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>14</v>
@@ -2224,7 +2227,7 @@
         <v>17</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>19</v>
@@ -2235,13 +2238,13 @@
         <v>95</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>14</v>
@@ -2255,25 +2258,25 @@
       <c r="H47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>18</v>
+      <c r="I47" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>14</v>
@@ -2281,14 +2284,14 @@
       <c r="F48" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="G48" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>23</v>
+      <c r="I48" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>19</v>
@@ -2299,13 +2302,13 @@
         <v>95</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>14</v>
@@ -2320,7 +2323,7 @@
         <v>17</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>19</v>
@@ -2331,13 +2334,13 @@
         <v>95</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>14</v>
@@ -2351,25 +2354,25 @@
       <c r="H50" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I50" s="13" t="s">
-        <v>115</v>
+      <c r="I50" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>14</v>
@@ -2377,14 +2380,14 @@
       <c r="F51" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="G51" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I51" s="13" t="s">
-        <v>117</v>
+      <c r="I51" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>19</v>
@@ -2395,25 +2398,28 @@
         <v>95</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>106</v>
+        <v>14</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>19</v>
@@ -2424,54 +2430,60 @@
         <v>95</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="H53" s="12" t="s">
-        <v>106</v>
+        <v>14</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="H54" s="12" t="s">
-        <v>106</v>
+        <v>14</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>19</v>
@@ -2482,10 +2494,10 @@
         <v>95</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>134</v>
@@ -2493,49 +2505,136 @@
       <c r="E55" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F55" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G55" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="H55" s="12" t="s">
-        <v>106</v>
+      <c r="G55" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="H56" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E57" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E58" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="B59" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G56" s="10" t="s">
+      <c r="C59" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J56" s="11" t="s">
+      <c r="F59" s="13" t="s">
         <v>144</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J59" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small mods: imp_spat_db='GO' to 'GO-Maps'
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -244,7 +244,7 @@
     <t xml:space="preserve">CRED</t>
   </si>
   <si>
-    <t xml:space="preserve">EM-DAT</t>
+    <t xml:space="preserve">EMDAT</t>
   </si>
   <si>
     <t xml:space="preserve">AID.Contribution</t>
@@ -488,7 +488,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -536,12 +536,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -606,7 +600,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -652,10 +646,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -663,7 +653,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -746,8 +736,8 @@
   </sheetPr>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A428" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B461" activeCellId="0" sqref="B461"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1872,10 +1862,10 @@
       <c r="F35" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H35" s="11" t="s">
         <v>110</v>
       </c>
       <c r="I35" s="3" t="s">
@@ -2038,7 +2028,7 @@
       <c r="H40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I40" s="13" t="s">
+      <c r="I40" s="12" t="s">
         <v>117</v>
       </c>
       <c r="J40" s="1" t="s">
@@ -2070,7 +2060,7 @@
       <c r="H41" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="I41" s="12" t="s">
         <v>119</v>
       </c>
       <c r="J41" s="1" t="s">
@@ -2230,7 +2220,7 @@
       <c r="H46" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I46" s="13" t="s">
+      <c r="I46" s="12" t="s">
         <v>117</v>
       </c>
       <c r="J46" s="1" t="s">
@@ -2262,7 +2252,7 @@
       <c r="H47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I47" s="13" t="s">
+      <c r="I47" s="12" t="s">
         <v>119</v>
       </c>
       <c r="J47" s="1" t="s">
@@ -2422,7 +2412,7 @@
       <c r="H52" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I52" s="13" t="s">
+      <c r="I52" s="12" t="s">
         <v>117</v>
       </c>
       <c r="J52" s="1" t="s">
@@ -2454,7 +2444,7 @@
       <c r="H53" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I53" s="13" t="s">
+      <c r="I53" s="12" t="s">
         <v>119</v>
       </c>
       <c r="J53" s="1" t="s">
@@ -2483,7 +2473,7 @@
       <c r="G54" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H54" s="12" t="s">
+      <c r="H54" s="11" t="s">
         <v>110</v>
       </c>
       <c r="J54" s="1" t="s">
@@ -2512,7 +2502,7 @@
       <c r="G55" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H55" s="12" t="s">
+      <c r="H55" s="11" t="s">
         <v>110</v>
       </c>
       <c r="J55" s="1" t="s">
@@ -2541,7 +2531,7 @@
       <c r="G56" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="H56" s="11" t="s">
         <v>110</v>
       </c>
       <c r="J56" s="1" t="s">
@@ -2570,7 +2560,7 @@
       <c r="G57" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H57" s="12" t="s">
+      <c r="H57" s="11" t="s">
         <v>110</v>
       </c>
       <c r="J57" s="1" t="s">
@@ -2593,7 +2583,7 @@
       <c r="E58" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="13" t="s">
         <v>142</v>
       </c>
       <c r="G58" s="9" t="s">

</xml_diff>

<commit_message>
minor mod changing 'in need' for EM-DAT impact taxonomy
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/Taxonomies/MostlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="146">
   <si>
     <t xml:space="preserve">imp_src_orgtype</t>
   </si>
@@ -265,7 +265,7 @@
     <t xml:space="preserve">No.Affected</t>
   </si>
   <si>
-    <t xml:space="preserve">imptypneed</t>
+    <t xml:space="preserve">imptypaffe</t>
   </si>
   <si>
     <t xml:space="preserve">No.Homeless</t>
@@ -275,9 +275,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total.Affected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imptypaffe</t>
   </si>
   <si>
     <t xml:space="preserve">Reconstruction.Costs</t>
@@ -659,12 +656,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -729,30 +726,136 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,7 +1588,7 @@
         <v>17</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>19</v>
@@ -1502,16 +1605,16 @@
         <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>43</v>
@@ -1534,16 +1637,16 @@
         <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>43</v>
@@ -1566,16 +1669,16 @@
         <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>43</v>
@@ -1598,16 +1701,16 @@
         <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>43</v>
@@ -1630,16 +1733,16 @@
         <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>43</v>
@@ -1662,16 +1765,16 @@
         <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>43</v>
@@ -1685,31 +1788,31 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>19</v>
@@ -1717,16 +1820,16 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>14</v>
@@ -1741,7 +1844,7 @@
         <v>17</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>19</v>
@@ -1749,16 +1852,16 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>14</v>
@@ -1773,7 +1876,7 @@
         <v>17</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>19</v>
@@ -1781,17 +1884,17 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="C33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E33" s="3" t="s">
         <v>14</v>
       </c>
@@ -1805,7 +1908,7 @@
         <v>17</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>19</v>
@@ -1813,31 +1916,31 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>19</v>
@@ -1845,16 +1948,16 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>40</v>
@@ -1863,10 +1966,10 @@
         <v>70</v>
       </c>
       <c r="G35" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>44</v>
@@ -1877,16 +1980,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>14</v>
@@ -1909,16 +2012,16 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>14</v>
@@ -1941,16 +2044,16 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>14</v>
@@ -1973,16 +2076,16 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>14</v>
@@ -1997,7 +2100,7 @@
         <v>17</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>19</v>
@@ -2005,31 +2108,31 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>19</v>
@@ -2037,31 +2140,31 @@
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>19</v>
@@ -2069,16 +2172,16 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>14</v>
@@ -2101,16 +2204,16 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>14</v>
@@ -2133,16 +2236,16 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>14</v>
@@ -2165,16 +2268,16 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>14</v>
@@ -2189,7 +2292,7 @@
         <v>17</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>19</v>
@@ -2197,16 +2300,16 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>14</v>
@@ -2221,7 +2324,7 @@
         <v>17</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>19</v>
@@ -2229,16 +2332,16 @@
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>14</v>
@@ -2253,7 +2356,7 @@
         <v>17</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>19</v>
@@ -2261,16 +2364,16 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>14</v>
@@ -2293,16 +2396,16 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>14</v>
@@ -2325,16 +2428,16 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>14</v>
@@ -2357,16 +2460,16 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>14</v>
@@ -2381,7 +2484,7 @@
         <v>17</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>19</v>
@@ -2389,16 +2492,16 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>14</v>
@@ -2413,7 +2516,7 @@
         <v>17</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>19</v>
@@ -2421,16 +2524,16 @@
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>14</v>
@@ -2445,7 +2548,7 @@
         <v>17</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>19</v>
@@ -2453,16 +2556,16 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>40</v>
@@ -2471,10 +2574,10 @@
         <v>70</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>19</v>
@@ -2482,16 +2585,16 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>40</v>
@@ -2500,10 +2603,10 @@
         <v>70</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>19</v>
@@ -2511,16 +2614,16 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>40</v>
@@ -2529,10 +2632,10 @@
         <v>70</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>19</v>
@@ -2540,16 +2643,16 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>40</v>
@@ -2558,10 +2661,10 @@
         <v>70</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>19</v>
@@ -2569,40 +2672,40 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="F58" s="13" t="s">
+      <c r="G58" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="H58" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="J58" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="J58" s="10" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>